<commit_message>
Report: Update latency vs. resource
</commit_message>
<xml_diff>
--- a/report/data/summary.xlsx
+++ b/report/data/summary.xlsx
@@ -1644,7 +1644,17 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="x"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -1755,12 +1765,25 @@
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
+              <a:prstDash val="solid"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -1876,7 +1899,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="triangle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -1992,7 +2027,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="diamond"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -2323,7 +2370,62 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Resource usage</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2391,8 +2493,8 @@
           <c:yMode val="edge"/>
           <c:x val="6.5985336217466717E-2"/>
           <c:y val="3.6133694670280035E-3"/>
-          <c:w val="0.85969846361797364"/>
-          <c:h val="7.4252273698345847E-2"/>
+          <c:w val="0.84188103153342153"/>
+          <c:h val="7.6936090819972811E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -3617,15 +3719,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>371474</xdr:colOff>
+      <xdr:colOff>371476</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>34</xdr:col>
-      <xdr:colOff>38099</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4044,7 +4146,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AH26" sqref="AH26"/>
+      <selection pane="bottomRight" activeCell="AJ26" sqref="AJ26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Report: Update throughput data
</commit_message>
<xml_diff>
--- a/report/data/summary.xlsx
+++ b/report/data/summary.xlsx
@@ -2827,37 +2827,37 @@
                   <c:v>0.30107733000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.3627093155000001</c:v>
+                  <c:v>1.3624277415000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.3427949500000003E-2</c:v>
+                  <c:v>1.31428085E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.1823369999999996E-3</c:v>
+                  <c:v>7.8995390000000006E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.3162080000000002E-3</c:v>
+                  <c:v>6.031718000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.4691309999999995E-3</c:v>
+                  <c:v>5.1845225000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.9570489999999998E-3</c:v>
+                  <c:v>4.6715554999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.6165924999999998E-3</c:v>
+                  <c:v>4.3301284999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.4431925000000001E-3</c:v>
+                  <c:v>4.1598469999999995E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.2758689999999999E-3</c:v>
+                  <c:v>3.9916774999999996E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.0494240000000003E-3</c:v>
+                  <c:v>3.7683300000000003E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.9765750000000004E-3</c:v>
+                  <c:v>3.6956040000000003E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3130,34 +3130,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>148.94306833668085</c:v>
+                  <c:v>152.17447625444746</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>244.42894493345852</c:v>
+                  <c:v>253.17933109767543</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>316.64568361269926</c:v>
+                  <c:v>331.58048834511152</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>365.68880869739638</c:v>
+                  <c:v>385.76358767851809</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>403.46585236498572</c:v>
+                  <c:v>428.12292393829</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>433.21995606066594</c:v>
+                  <c:v>461.88005737012196</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>450.12679509159238</c:v>
+                  <c:v>480.78691355715733</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>467.74117729051102</c:v>
+                  <c:v>501.04248151309821</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>493.89740368012826</c:v>
+                  <c:v>530.73908070683831</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>502.94537384558311</c:v>
+                  <c:v>541.18352507465625</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6905,7 +6905,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AO18" sqref="AO18"/>
+      <selection pane="bottomRight" activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8751,12 +8751,12 @@
         <v>unopt</v>
       </c>
       <c r="T17" s="5">
-        <f>M2</f>
-        <v>1.3627093155000001</v>
+        <f>V2*(1/$G$15)</f>
+        <v>1.3624277415000001</v>
       </c>
       <c r="V17" s="6">
         <f t="shared" si="0"/>
-        <v>1.4676644367593301</v>
+        <v>1.4679677601089127</v>
       </c>
     </row>
     <row r="18" spans="12:22" x14ac:dyDescent="0.25">
@@ -8773,12 +8773,12 @@
         <v>1</v>
       </c>
       <c r="T18" s="5">
-        <f>M3</f>
-        <v>1.3427949500000003E-2</v>
+        <f>V3*(1/$G$15)</f>
+        <v>1.31428085E-2</v>
       </c>
       <c r="V18" s="6">
         <f t="shared" si="0"/>
-        <v>148.94306833668085</v>
+        <v>152.17447625444746</v>
       </c>
     </row>
     <row r="19" spans="12:22" x14ac:dyDescent="0.25">
@@ -8793,12 +8793,12 @@
         <v>2</v>
       </c>
       <c r="T19" s="5">
-        <f>M4</f>
-        <v>8.1823369999999996E-3</v>
+        <f t="shared" ref="T19:T27" si="1">V4*(1/$G$15)</f>
+        <v>7.8995390000000006E-3</v>
       </c>
       <c r="V19" s="6">
         <f t="shared" si="0"/>
-        <v>244.42894493345852</v>
+        <v>253.17933109767543</v>
       </c>
     </row>
     <row r="20" spans="12:22" x14ac:dyDescent="0.25">
@@ -8807,12 +8807,12 @@
         <v>3</v>
       </c>
       <c r="T20" s="5">
-        <f>M5</f>
-        <v>6.3162080000000002E-3</v>
+        <f t="shared" si="1"/>
+        <v>6.031718000000001E-3</v>
       </c>
       <c r="V20" s="6">
         <f t="shared" si="0"/>
-        <v>316.64568361269926</v>
+        <v>331.58048834511152</v>
       </c>
     </row>
     <row r="21" spans="12:22" x14ac:dyDescent="0.25">
@@ -8821,12 +8821,12 @@
         <v>4</v>
       </c>
       <c r="T21" s="5">
-        <f>M6</f>
-        <v>5.4691309999999995E-3</v>
+        <f t="shared" si="1"/>
+        <v>5.1845225000000002E-3</v>
       </c>
       <c r="V21" s="6">
         <f t="shared" si="0"/>
-        <v>365.68880869739638</v>
+        <v>385.76358767851809</v>
       </c>
     </row>
     <row r="22" spans="12:22" x14ac:dyDescent="0.25">
@@ -8835,12 +8835,12 @@
         <v>5</v>
       </c>
       <c r="T22" s="5">
-        <f>M7</f>
-        <v>4.9570489999999998E-3</v>
+        <f t="shared" si="1"/>
+        <v>4.6715554999999997E-3</v>
       </c>
       <c r="V22" s="6">
         <f t="shared" si="0"/>
-        <v>403.46585236498572</v>
+        <v>428.12292393829</v>
       </c>
     </row>
     <row r="23" spans="12:22" x14ac:dyDescent="0.25">
@@ -8849,12 +8849,12 @@
         <v>6</v>
       </c>
       <c r="T23" s="5">
-        <f>M8</f>
-        <v>4.6165924999999998E-3</v>
+        <f t="shared" si="1"/>
+        <v>4.3301284999999997E-3</v>
       </c>
       <c r="V23" s="6">
         <f t="shared" si="0"/>
-        <v>433.21995606066594</v>
+        <v>461.88005737012196</v>
       </c>
     </row>
     <row r="24" spans="12:22" x14ac:dyDescent="0.25">
@@ -8863,12 +8863,12 @@
         <v>7</v>
       </c>
       <c r="T24" s="5">
-        <f>M9</f>
-        <v>4.4431925000000001E-3</v>
+        <f t="shared" si="1"/>
+        <v>4.1598469999999995E-3</v>
       </c>
       <c r="V24" s="6">
         <f t="shared" si="0"/>
-        <v>450.12679509159238</v>
+        <v>480.78691355715733</v>
       </c>
     </row>
     <row r="25" spans="12:22" x14ac:dyDescent="0.25">
@@ -8877,12 +8877,12 @@
         <v>8</v>
       </c>
       <c r="T25" s="5">
-        <f>M10</f>
-        <v>4.2758689999999999E-3</v>
+        <f t="shared" si="1"/>
+        <v>3.9916774999999996E-3</v>
       </c>
       <c r="V25" s="6">
         <f t="shared" si="0"/>
-        <v>467.74117729051102</v>
+        <v>501.04248151309821</v>
       </c>
     </row>
     <row r="26" spans="12:22" x14ac:dyDescent="0.25">
@@ -8891,12 +8891,12 @@
         <v>9</v>
       </c>
       <c r="T26" s="5">
-        <f>M11</f>
-        <v>4.0494240000000003E-3</v>
+        <f t="shared" si="1"/>
+        <v>3.7683300000000003E-3</v>
       </c>
       <c r="V26" s="6">
         <f t="shared" si="0"/>
-        <v>493.89740368012826</v>
+        <v>530.73908070683831</v>
       </c>
     </row>
     <row r="27" spans="12:22" x14ac:dyDescent="0.25">
@@ -8905,12 +8905,12 @@
         <v>10</v>
       </c>
       <c r="T27" s="5">
-        <f>M12</f>
-        <v>3.9765750000000004E-3</v>
+        <f t="shared" si="1"/>
+        <v>3.6956040000000003E-3</v>
       </c>
       <c r="V27" s="6">
         <f t="shared" si="0"/>
-        <v>502.94537384558311</v>
+        <v>541.18352507465625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update figures to include data labels
</commit_message>
<xml_diff>
--- a/report/data/summary.xlsx
+++ b/report/data/summary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Unroll</t>
   </si>
@@ -155,6 +155,9 @@
     <t>iTotalCF</t>
   </si>
   <si>
+    <t>Column1</t>
+  </si>
+  <si>
     <t>pollingT</t>
   </si>
   <si>
@@ -183,6 +186,18 @@
   </si>
   <si>
     <t>Throughput</t>
+  </si>
+  <si>
+    <t>tData</t>
+  </si>
+  <si>
+    <t>tStart</t>
+  </si>
+  <si>
+    <t>tResult</t>
+  </si>
+  <si>
+    <t>1126587</t>
   </si>
 </sst>
 </file>
@@ -235,12 +250,30 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="42">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000E+00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -570,28 +603,28 @@
                   <c:v>136302019.80000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1367113.7874999999</c:v>
+                  <c:v>1367113.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>841941.43750000012</c:v>
+                  <c:v>841941.40000000014</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>666875.68750000012</c:v>
+                  <c:v>666875.65000000014</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>580938.88750000007</c:v>
+                  <c:v>580938.85000000009</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>527703.58750000002</c:v>
+                  <c:v>527703.55000000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>493147.03750000009</c:v>
+                  <c:v>493147.00000000012</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>468309.43750000012</c:v>
+                  <c:v>468309.4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>450912.88750000007</c:v>
+                  <c:v>450912.85000000009</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>436073.55</c:v>
@@ -1573,6 +1606,64 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$2:$A$12</c:f>
@@ -1665,7 +1756,7 @@
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -1715,6 +1806,9 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$2:$A$12</c:f>
@@ -1844,6 +1938,9 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$2:$A$12</c:f>
@@ -1972,6 +2069,9 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$2:$A$12</c:f>
@@ -2100,6 +2200,9 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$2:$A$12</c:f>
@@ -2192,7 +2295,7 @@
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -2830,34 +2933,34 @@
                   <c:v>1.3624277415000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.31428085E-2</c:v>
+                  <c:v>13.142808500000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.8995390000000006E-3</c:v>
+                  <c:v>7.8995390000000008</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.031718000000001E-3</c:v>
+                  <c:v>6.0317180000000006</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.1845225000000002E-3</c:v>
+                  <c:v>5.1845224999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.6715554999999997E-3</c:v>
+                  <c:v>4.6715554999999993</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.3301284999999997E-3</c:v>
+                  <c:v>4.3301284999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.1598469999999995E-3</c:v>
+                  <c:v>4.1598469999999992</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.9916774999999996E-3</c:v>
+                  <c:v>3.9916774999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.7683300000000003E-3</c:v>
+                  <c:v>3.7683300000000002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.6956040000000003E-3</c:v>
+                  <c:v>3.6956040000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3084,6 +3187,65 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$R$18:$R$27</c:f>
@@ -3130,16 +3292,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>152.17447625444746</c:v>
+                  <c:v>152.17447625444743</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>253.17933109767543</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>331.58048834511152</c:v>
+                  <c:v>331.58048834511158</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>385.76358767851809</c:v>
+                  <c:v>385.76358767851815</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>428.12292393829</c:v>
@@ -3148,7 +3310,7 @@
                   <c:v>461.88005737012196</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>480.78691355715733</c:v>
+                  <c:v>480.78691355715739</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>501.04248151309821</c:v>
@@ -4119,6 +4281,1117 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Y$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>tData</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$R$15:$R$27</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$R$18:$R$27</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$Y$15:$Y$27</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$Y$18:$Y$27</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0" formatCode="0.000E+00">
+                  <c:v>1.6451210000000001</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="0.000E+00">
+                  <c:v>1.6441805000000003</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.000E+00">
+                  <c:v>1.6447400000000001</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.000E+00">
+                  <c:v>1.6450835000000001</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.000E+00">
+                  <c:v>1.6452665</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.000E+00">
+                  <c:v>1.6442419999999998</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.000E+00">
+                  <c:v>1.6441325</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.000E+00">
+                  <c:v>1.6453100000000001</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.000E+00">
+                  <c:v>1.6442640000000004</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.000E+00">
+                  <c:v>1.6456589999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-470E-4AE5-AA30-D569EA8AEF2F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Z$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>tStart</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$R$15:$R$27</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$R$18:$R$27</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$Z$15:$Z$27</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$Z$18:$Z$27</c:f>
+              <c:numCache>
+                <c:formatCode>0.000E+00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.40040249999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.40118250000000011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.40066200000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.40116000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.40041450000000006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.40090050000000005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.40116450000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.40083000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.40022249999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.39971550000000006</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-470E-4AE5-AA30-D569EA8AEF2F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AC$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>tResult</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$R$15:$R$27</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$R$18:$R$27</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$AC$15:$AC$27</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$AC$18:$AC$27</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0" formatCode="0.000E+00">
+                  <c:v>11.097284999999999</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="0.000E+00">
+                  <c:v>5.8541759999999998</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.000E+00">
+                  <c:v>3.986316</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.000E+00">
+                  <c:v>3.1382790000000003</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.000E+00">
+                  <c:v>2.6258745000000001</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.000E+00">
+                  <c:v>2.284986</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.000E+00">
+                  <c:v>2.1145500000000004</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.000E+00">
+                  <c:v>1.9455375000000004</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.000E+00">
+                  <c:v>1.7238435000000001</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.000E+00">
+                  <c:v>1.6502295000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-470E-4AE5-AA30-D569EA8AEF2F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="50"/>
+        <c:overlap val="100"/>
+        <c:axId val="473788000"/>
+        <c:axId val="478665792"/>
+      </c:barChart>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AA$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1126587</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$R$15:$R$27</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$R$18:$R$27</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>double</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>fixed</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>unopt</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$AA$15:$AA$27</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$AA$18:$AA$27</c:f>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-470E-4AE5-AA30-D569EA8AEF2F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AB$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Column1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$R$15:$R$27</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$R$18:$R$27</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>double</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>fixed</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>unopt</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$AB$15:$AB$27</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$AB$18:$AB$27</c:f>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-470E-4AE5-AA30-D569EA8AEF2F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="473788000"/>
+        <c:axId val="478665792"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$T$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="15875" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="10"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>3</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>4</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>5</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>6</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>7</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>8</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>9</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:autoCat val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$T$15:$T$27</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$T$18:$T$27</c:f>
+              <c:numCache>
+                <c:formatCode>0.000E+00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>13.142808500000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.8995390000000008</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.0317180000000006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.1845224999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.6715554999999993</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.3301284999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.1598469999999992</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.9916774999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.7683300000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.6956040000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-470E-4AE5-AA30-D569EA8AEF2F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="473788000"/>
+        <c:axId val="478665792"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="473788000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Loop unroll factor</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="478665792"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="478665792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="473788000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1200" b="0" i="0">
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup paperSize="9" orientation="landscape"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -4279,6 +5552,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -6324,6 +7637,511 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -6457,16 +8275,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>352424</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>161924</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6491,6 +8309,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>447676</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEEF61A7-46DA-438B-A02F-97FC45206C7D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6507,78 +8361,78 @@
     <tableColumn id="7" name="DSP"/>
     <tableColumn id="8" name="FF"/>
     <tableColumn id="9" name="LUT"/>
-    <tableColumn id="14" name="polling" dataDxfId="35"/>
-    <tableColumn id="24" name="pollingC" dataDxfId="34">
+    <tableColumn id="14" name="polling" dataDxfId="41"/>
+    <tableColumn id="24" name="pollingC" dataDxfId="40">
       <calculatedColumnFormula>IF(Table1[[#This Row],[pData]]&gt;1100000,Table1[[#This Row],[polling]]-$N$16,Table1[[#This Row],[polling]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" name="pollingCF" dataDxfId="33">
+    <tableColumn id="28" name="pollingCF" dataDxfId="39">
       <calculatedColumnFormula>Table1[[#This Row],[pollingC]]/$G$14*$G$15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="39" name="pollingT" dataDxfId="7">
+    <tableColumn id="39" name="pollingT" dataDxfId="13">
       <calculatedColumnFormula>Table1[[#This Row],[pollingCF]]*(1/$G$15)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="pData" dataDxfId="32"/>
-    <tableColumn id="22" name="pDataC" dataDxfId="31">
+    <tableColumn id="17" name="pData" dataDxfId="38"/>
+    <tableColumn id="22" name="pDataC" dataDxfId="37">
       <calculatedColumnFormula>IF(Table1[[#This Row],[pData]]&gt;1100000,Table1[[#This Row],[pData]]-$N$16,Table1[[#This Row],[pData]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" name="pDataCF" dataDxfId="30">
+    <tableColumn id="29" name="pDataCF" dataDxfId="36">
       <calculatedColumnFormula>Table1[[#This Row],[pDataC]]/$G$14*$G$15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="pStart" dataDxfId="29"/>
-    <tableColumn id="30" name="pStartF" dataDxfId="28">
+    <tableColumn id="16" name="pStart" dataDxfId="35"/>
+    <tableColumn id="30" name="pStartF" dataDxfId="34">
       <calculatedColumnFormula>Table1[[#This Row],[pStart]]/$G$14*$G$15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="pResult" dataDxfId="27"/>
-    <tableColumn id="31" name="pResultF" dataDxfId="26">
+    <tableColumn id="15" name="pResult" dataDxfId="33"/>
+    <tableColumn id="31" name="pResultF" dataDxfId="32">
       <calculatedColumnFormula>Table1[[#This Row],[pResult]]/$G$14*$G$15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" name="pTotalC" dataDxfId="25">
+    <tableColumn id="26" name="pTotalC" dataDxfId="31">
       <calculatedColumnFormula>SUM(Table1[[#This Row],[pDataC]],Table1[[#This Row],[pStart]],Table1[[#This Row],[pResult]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="32" name="pTotalCF" dataDxfId="24">
+    <tableColumn id="32" name="pTotalCF" dataDxfId="30">
       <calculatedColumnFormula>Table1[[#This Row],[pTotalC]]/$G$14*$G$15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="interrupt" dataDxfId="23"/>
-    <tableColumn id="25" name="interruptC" dataDxfId="22">
+    <tableColumn id="18" name="interrupt" dataDxfId="29"/>
+    <tableColumn id="25" name="interruptC" dataDxfId="28">
       <calculatedColumnFormula>IF(Table1[[#This Row],[iData]]&gt;1100000,Table1[[#This Row],[interrupt]]-$AA$16,Table1[[#This Row],[interrupt]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="33" name="interruptCF" dataDxfId="21">
+    <tableColumn id="33" name="interruptCF" dataDxfId="27">
       <calculatedColumnFormula>Table1[[#This Row],[interruptC]]/$G$14*$G$15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="40" name="interruptT" dataDxfId="6">
+    <tableColumn id="40" name="interruptT" dataDxfId="12">
       <calculatedColumnFormula>Table1[[#This Row],[interruptCF]]*(1/$G$15)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="iData" dataDxfId="20"/>
-    <tableColumn id="23" name="iDataC" dataDxfId="19">
+    <tableColumn id="21" name="iData" dataDxfId="26"/>
+    <tableColumn id="23" name="iDataC" dataDxfId="25">
       <calculatedColumnFormula>IF(Table1[[#This Row],[iData]]&gt;1100000,Table1[[#This Row],[iData]]-$AA$16,Table1[[#This Row],[iData]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" name="iDataCF" dataDxfId="18">
+    <tableColumn id="34" name="iDataCF" dataDxfId="24">
       <calculatedColumnFormula>Table1[[#This Row],[iDataC]]/$G$14*$G$15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="iStart" dataDxfId="17"/>
-    <tableColumn id="35" name="iStartF" dataDxfId="16">
+    <tableColumn id="20" name="iStart" dataDxfId="23"/>
+    <tableColumn id="35" name="iStartF" dataDxfId="22">
       <calculatedColumnFormula>Table1[[#This Row],[iStart]]/$G$14*$G$15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="iResult" dataDxfId="15"/>
-    <tableColumn id="36" name="iResultF" dataDxfId="14">
+    <tableColumn id="19" name="iResult" dataDxfId="21"/>
+    <tableColumn id="36" name="iResultF" dataDxfId="20">
       <calculatedColumnFormula>Table1[[#This Row],[iResult]]/$G$14*$G$15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="iTotalC" dataDxfId="13">
+    <tableColumn id="27" name="iTotalC" dataDxfId="19">
       <calculatedColumnFormula>SUM(Table1[[#This Row],[iDataC]],Table1[[#This Row],[iStart]],Table1[[#This Row],[iResult]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="37" name="iTotalCF" dataDxfId="12">
+    <tableColumn id="37" name="iTotalCF" dataDxfId="18">
       <calculatedColumnFormula>Table1[[#This Row],[iTotalC]]/$G$14*$G$15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="BRAM %" dataDxfId="11">
+    <tableColumn id="10" name="BRAM %" dataDxfId="17">
       <calculatedColumnFormula>Table1[BRAM]/280</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="DSP %" dataDxfId="10">
+    <tableColumn id="11" name="DSP %" dataDxfId="16">
       <calculatedColumnFormula>Table1[DSP]/220</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="FF %" dataDxfId="9">
+    <tableColumn id="12" name="FF %" dataDxfId="15">
       <calculatedColumnFormula>Table1[FF]/106400</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="LUT %" dataDxfId="8">
+    <tableColumn id="13" name="LUT %" dataDxfId="14">
       <calculatedColumnFormula>Table1[LUT]/53200</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -6587,16 +8441,30 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="R14:V27" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="R14:V27" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="R14:V27"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Type" dataDxfId="5"/>
-    <tableColumn id="2" name="Column2" dataDxfId="4"/>
-    <tableColumn id="3" name="Time" dataDxfId="3"/>
-    <tableColumn id="4" name="Column4" dataDxfId="2"/>
-    <tableColumn id="5" name="Throughput" dataDxfId="1">
-      <calculatedColumnFormula>2000/T15/1000</calculatedColumnFormula>
+    <tableColumn id="1" name="Type" dataDxfId="11"/>
+    <tableColumn id="2" name="Column2" dataDxfId="10"/>
+    <tableColumn id="3" name="Time" dataDxfId="9"/>
+    <tableColumn id="4" name="Column4" dataDxfId="8"/>
+    <tableColumn id="5" name="Throughput" dataDxfId="0">
+      <calculatedColumnFormula>2000/T15</calculatedColumnFormula>
     </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="Y14:AC27" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="Y14:AC27"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="tData" dataDxfId="6"/>
+    <tableColumn id="2" name="tStart" dataDxfId="5"/>
+    <tableColumn id="3" name="1126587" dataDxfId="4"/>
+    <tableColumn id="4" name="Column1" dataDxfId="3"/>
+    <tableColumn id="5" name="tResult" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6902,10 +8770,10 @@
   <dimension ref="A1:AY27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="L22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T17" sqref="T17"/>
+      <selection pane="bottomRight" activeCell="AC45" sqref="AC45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6992,7 +8860,7 @@
         <v>33</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>15</v>
@@ -7031,7 +8899,7 @@
         <v>38</v>
       </c>
       <c r="Z1" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AA1" s="2" t="s">
         <v>18</v>
@@ -7073,7 +8941,7 @@
         <v>12</v>
       </c>
       <c r="AY1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:51" x14ac:dyDescent="0.25">
@@ -7298,26 +9166,26 @@
       </c>
       <c r="X3" s="2">
         <f>IF(Table1[[#This Row],[iData]]&gt;1100000,Table1[[#This Row],[interrupt]]-$AA$16,Table1[[#This Row],[interrupt]])</f>
-        <v>9114091.916666666</v>
+        <v>9114091.666666666</v>
       </c>
       <c r="Y3" s="2">
         <f>Table1[[#This Row],[interruptC]]/$G$14*$G$15</f>
-        <v>1367113.7874999999</v>
+        <v>1367113.75</v>
       </c>
       <c r="Z3" s="5">
         <f>Table1[[#This Row],[interruptCF]]*(1/$G$15)</f>
-        <v>1.3671137874999999E-2</v>
+        <v>1.36711375E-2</v>
       </c>
       <c r="AA3" s="2">
         <v>1127105</v>
       </c>
       <c r="AB3" s="2">
         <f>IF(Table1[[#This Row],[iData]]&gt;1100000,Table1[[#This Row],[iData]]-$AA$16,Table1[[#This Row],[iData]])</f>
-        <v>1090327.9166666667</v>
+        <v>1090327.6666666667</v>
       </c>
       <c r="AC3" s="2">
         <f>Table1[[#This Row],[iDataC]]/$G$14*$G$15</f>
-        <v>163549.18750000003</v>
+        <v>163549.15000000002</v>
       </c>
       <c r="AD3" s="2">
         <v>262349</v>
@@ -7335,11 +9203,11 @@
       </c>
       <c r="AH3" s="2">
         <f>SUM(Table1[[#This Row],[iDataC]],Table1[[#This Row],[iStart]],Table1[[#This Row],[iResult]])</f>
-        <v>8932844.916666666</v>
+        <v>8932844.666666666</v>
       </c>
       <c r="AI3" s="2">
         <f>Table1[[#This Row],[iTotalC]]/$G$14*$G$15</f>
-        <v>1339926.7374999998</v>
+        <v>1339926.7</v>
       </c>
       <c r="AJ3" s="1">
         <f>Table1[BRAM]/280</f>
@@ -7439,26 +9307,26 @@
       </c>
       <c r="X4" s="2">
         <f>IF(Table1[[#This Row],[iData]]&gt;1100000,Table1[[#This Row],[interrupt]]-$AA$16,Table1[[#This Row],[interrupt]])</f>
-        <v>5612942.916666667</v>
+        <v>5612942.666666667</v>
       </c>
       <c r="Y4" s="2">
         <f>Table1[[#This Row],[interruptC]]/$G$14*$G$15</f>
-        <v>841941.43750000012</v>
+        <v>841941.40000000014</v>
       </c>
       <c r="Z4" s="5">
         <f>Table1[[#This Row],[interruptCF]]*(1/$G$15)</f>
-        <v>8.4194143750000016E-3</v>
+        <v>8.4194140000000018E-3</v>
       </c>
       <c r="AA4" s="2">
         <v>1126676</v>
       </c>
       <c r="AB4" s="2">
         <f>IF(Table1[[#This Row],[iData]]&gt;1100000,Table1[[#This Row],[iData]]-$AA$16,Table1[[#This Row],[iData]])</f>
-        <v>1089898.9166666667</v>
+        <v>1089898.6666666667</v>
       </c>
       <c r="AC4" s="2">
         <f>Table1[[#This Row],[iDataC]]/$G$14*$G$15</f>
-        <v>163484.83750000002</v>
+        <v>163484.80000000002</v>
       </c>
       <c r="AD4" s="2">
         <v>262946</v>
@@ -7476,11 +9344,11 @@
       </c>
       <c r="AH4" s="2">
         <f>SUM(Table1[[#This Row],[iDataC]],Table1[[#This Row],[iStart]],Table1[[#This Row],[iResult]])</f>
-        <v>5432288.916666667</v>
+        <v>5432288.666666667</v>
       </c>
       <c r="AI4" s="2">
         <f>Table1[[#This Row],[iTotalC]]/$G$14*$G$15</f>
-        <v>814843.33750000014</v>
+        <v>814843.30000000016</v>
       </c>
       <c r="AJ4" s="1">
         <f>Table1[BRAM]/280</f>
@@ -7580,26 +9448,26 @@
       </c>
       <c r="X5" s="2">
         <f>IF(Table1[[#This Row],[iData]]&gt;1100000,Table1[[#This Row],[interrupt]]-$AA$16,Table1[[#This Row],[interrupt]])</f>
-        <v>4445837.916666667</v>
+        <v>4445837.666666667</v>
       </c>
       <c r="Y5" s="2">
         <f>Table1[[#This Row],[interruptC]]/$G$14*$G$15</f>
-        <v>666875.68750000012</v>
+        <v>666875.65000000014</v>
       </c>
       <c r="Z5" s="5">
         <f>Table1[[#This Row],[interruptCF]]*(1/$G$15)</f>
-        <v>6.6687568750000009E-3</v>
+        <v>6.6687565000000011E-3</v>
       </c>
       <c r="AA5" s="2">
         <v>1125826</v>
       </c>
       <c r="AB5" s="2">
         <f>IF(Table1[[#This Row],[iData]]&gt;1100000,Table1[[#This Row],[iData]]-$AA$16,Table1[[#This Row],[iData]])</f>
-        <v>1089048.9166666667</v>
+        <v>1089048.6666666667</v>
       </c>
       <c r="AC5" s="2">
         <f>Table1[[#This Row],[iDataC]]/$G$14*$G$15</f>
-        <v>163357.33750000002</v>
+        <v>163357.30000000002</v>
       </c>
       <c r="AD5" s="2">
         <v>262582</v>
@@ -7617,11 +9485,11 @@
       </c>
       <c r="AH5" s="2">
         <f>SUM(Table1[[#This Row],[iDataC]],Table1[[#This Row],[iStart]],Table1[[#This Row],[iResult]])</f>
-        <v>4263516.916666667</v>
+        <v>4263516.666666667</v>
       </c>
       <c r="AI5" s="2">
         <f>Table1[[#This Row],[iTotalC]]/$G$14*$G$15</f>
-        <v>639527.53750000009</v>
+        <v>639527.50000000012</v>
       </c>
       <c r="AJ5" s="1">
         <f>Table1[BRAM]/280</f>
@@ -7721,26 +9589,26 @@
       </c>
       <c r="X6" s="2">
         <f>IF(Table1[[#This Row],[iData]]&gt;1100000,Table1[[#This Row],[interrupt]]-$AA$16,Table1[[#This Row],[interrupt]])</f>
-        <v>3872925.916666667</v>
+        <v>3872925.666666667</v>
       </c>
       <c r="Y6" s="2">
         <f>Table1[[#This Row],[interruptC]]/$G$14*$G$15</f>
-        <v>580938.88750000007</v>
+        <v>580938.85000000009</v>
       </c>
       <c r="Z6" s="5">
         <f>Table1[[#This Row],[interruptCF]]*(1/$G$15)</f>
-        <v>5.8093888750000008E-3</v>
+        <v>5.809388500000001E-3</v>
       </c>
       <c r="AA6" s="2">
         <v>1126660</v>
       </c>
       <c r="AB6" s="2">
         <f>IF(Table1[[#This Row],[iData]]&gt;1100000,Table1[[#This Row],[iData]]-$AA$16,Table1[[#This Row],[iData]])</f>
-        <v>1089882.9166666667</v>
+        <v>1089882.6666666667</v>
       </c>
       <c r="AC6" s="2">
         <f>Table1[[#This Row],[iDataC]]/$G$14*$G$15</f>
-        <v>163482.43750000003</v>
+        <v>163482.40000000002</v>
       </c>
       <c r="AD6" s="2">
         <v>263415</v>
@@ -7758,11 +9626,11 @@
       </c>
       <c r="AH6" s="2">
         <f>SUM(Table1[[#This Row],[iDataC]],Table1[[#This Row],[iStart]],Table1[[#This Row],[iResult]])</f>
-        <v>3690870.916666667</v>
+        <v>3690870.666666667</v>
       </c>
       <c r="AI6" s="2">
         <f>Table1[[#This Row],[iTotalC]]/$G$14*$G$15</f>
-        <v>553630.63750000007</v>
+        <v>553630.60000000009</v>
       </c>
       <c r="AJ6" s="1">
         <f>Table1[BRAM]/280</f>
@@ -7862,26 +9730,26 @@
       </c>
       <c r="X7" s="2">
         <f>IF(Table1[[#This Row],[iData]]&gt;1100000,Table1[[#This Row],[interrupt]]-$AA$16,Table1[[#This Row],[interrupt]])</f>
-        <v>3518023.916666667</v>
+        <v>3518023.666666667</v>
       </c>
       <c r="Y7" s="2">
         <f>Table1[[#This Row],[interruptC]]/$G$14*$G$15</f>
-        <v>527703.58750000002</v>
+        <v>527703.55000000005</v>
       </c>
       <c r="Z7" s="5">
         <f>Table1[[#This Row],[interruptCF]]*(1/$G$15)</f>
-        <v>5.2770358750000006E-3</v>
+        <v>5.2770355000000008E-3</v>
       </c>
       <c r="AA7" s="2">
         <v>1125638</v>
       </c>
       <c r="AB7" s="2">
         <f>IF(Table1[[#This Row],[iData]]&gt;1100000,Table1[[#This Row],[iData]]-$AA$16,Table1[[#This Row],[iData]])</f>
-        <v>1088860.9166666667</v>
+        <v>1088860.6666666667</v>
       </c>
       <c r="AC7" s="2">
         <f>Table1[[#This Row],[iDataC]]/$G$14*$G$15</f>
-        <v>163329.13750000004</v>
+        <v>163329.10000000003</v>
       </c>
       <c r="AD7" s="2">
         <v>262360</v>
@@ -7899,11 +9767,11 @@
       </c>
       <c r="AH7" s="2">
         <f>SUM(Table1[[#This Row],[iDataC]],Table1[[#This Row],[iStart]],Table1[[#This Row],[iResult]])</f>
-        <v>3337407.916666667</v>
+        <v>3337407.666666667</v>
       </c>
       <c r="AI7" s="2">
         <f>Table1[[#This Row],[iTotalC]]/$G$14*$G$15</f>
-        <v>500611.18750000012</v>
+        <v>500611.15000000014</v>
       </c>
       <c r="AJ7" s="1">
         <f>Table1[BRAM]/280</f>
@@ -8003,26 +9871,26 @@
       </c>
       <c r="X8" s="2">
         <f>IF(Table1[[#This Row],[iData]]&gt;1100000,Table1[[#This Row],[interrupt]]-$AA$16,Table1[[#This Row],[interrupt]])</f>
-        <v>3287646.916666667</v>
+        <v>3287646.666666667</v>
       </c>
       <c r="Y8" s="2">
         <f>Table1[[#This Row],[interruptC]]/$G$14*$G$15</f>
-        <v>493147.03750000009</v>
+        <v>493147.00000000012</v>
       </c>
       <c r="Z8" s="5">
         <f>Table1[[#This Row],[interruptCF]]*(1/$G$15)</f>
-        <v>4.931470375000001E-3</v>
+        <v>4.9314700000000012E-3</v>
       </c>
       <c r="AA8" s="2">
         <v>1126315</v>
       </c>
       <c r="AB8" s="2">
         <f>IF(Table1[[#This Row],[iData]]&gt;1100000,Table1[[#This Row],[iData]]-$AA$16,Table1[[#This Row],[iData]])</f>
-        <v>1089537.9166666667</v>
+        <v>1089537.6666666667</v>
       </c>
       <c r="AC8" s="2">
         <f>Table1[[#This Row],[iDataC]]/$G$14*$G$15</f>
-        <v>163430.68750000003</v>
+        <v>163430.65000000002</v>
       </c>
       <c r="AD8" s="2">
         <v>261956</v>
@@ -8040,11 +9908,11 @@
       </c>
       <c r="AH8" s="2">
         <f>SUM(Table1[[#This Row],[iDataC]],Table1[[#This Row],[iStart]],Table1[[#This Row],[iResult]])</f>
-        <v>3105189.916666667</v>
+        <v>3105189.666666667</v>
       </c>
       <c r="AI8" s="2">
         <f>Table1[[#This Row],[iTotalC]]/$G$14*$G$15</f>
-        <v>465778.4875000001</v>
+        <v>465778.45000000007</v>
       </c>
       <c r="AJ8" s="1">
         <f>Table1[BRAM]/280</f>
@@ -8144,26 +10012,26 @@
       </c>
       <c r="X9" s="2">
         <f>IF(Table1[[#This Row],[iData]]&gt;1100000,Table1[[#This Row],[interrupt]]-$AA$16,Table1[[#This Row],[interrupt]])</f>
-        <v>3122062.916666667</v>
+        <v>3122062.666666667</v>
       </c>
       <c r="Y9" s="2">
         <f>Table1[[#This Row],[interruptC]]/$G$14*$G$15</f>
-        <v>468309.43750000012</v>
+        <v>468309.4</v>
       </c>
       <c r="Z9" s="5">
         <f>Table1[[#This Row],[interruptCF]]*(1/$G$15)</f>
-        <v>4.6830943750000012E-3</v>
+        <v>4.6830940000000005E-3</v>
       </c>
       <c r="AA9" s="2">
         <v>1128502</v>
       </c>
       <c r="AB9" s="2">
         <f>IF(Table1[[#This Row],[iData]]&gt;1100000,Table1[[#This Row],[iData]]-$AA$16,Table1[[#This Row],[iData]])</f>
-        <v>1091724.9166666667</v>
+        <v>1091724.6666666667</v>
       </c>
       <c r="AC9" s="2">
         <f>Table1[[#This Row],[iDataC]]/$G$14*$G$15</f>
-        <v>163758.73750000002</v>
+        <v>163758.70000000001</v>
       </c>
       <c r="AD9" s="2">
         <v>262199</v>
@@ -8181,11 +10049,11 @@
       </c>
       <c r="AH9" s="2">
         <f>SUM(Table1[[#This Row],[iDataC]],Table1[[#This Row],[iStart]],Table1[[#This Row],[iResult]])</f>
-        <v>2939518.916666667</v>
+        <v>2939518.666666667</v>
       </c>
       <c r="AI9" s="2">
         <f>Table1[[#This Row],[iTotalC]]/$G$14*$G$15</f>
-        <v>440927.83750000008</v>
+        <v>440927.8000000001</v>
       </c>
       <c r="AJ9" s="1">
         <f>Table1[BRAM]/280</f>
@@ -8285,26 +10153,26 @@
       </c>
       <c r="X10" s="2">
         <f>IF(Table1[[#This Row],[iData]]&gt;1100000,Table1[[#This Row],[interrupt]]-$AA$16,Table1[[#This Row],[interrupt]])</f>
-        <v>3006085.916666667</v>
+        <v>3006085.666666667</v>
       </c>
       <c r="Y10" s="2">
         <f>Table1[[#This Row],[interruptC]]/$G$14*$G$15</f>
-        <v>450912.88750000007</v>
+        <v>450912.85000000009</v>
       </c>
       <c r="Z10" s="5">
         <f>Table1[[#This Row],[interruptCF]]*(1/$G$15)</f>
-        <v>4.5091288750000007E-3</v>
+        <v>4.5091285000000009E-3</v>
       </c>
       <c r="AA10" s="2">
         <v>1125972</v>
       </c>
       <c r="AB10" s="2">
         <f>IF(Table1[[#This Row],[iData]]&gt;1100000,Table1[[#This Row],[iData]]-$AA$16,Table1[[#This Row],[iData]])</f>
-        <v>1089194.9166666667</v>
+        <v>1089194.6666666667</v>
       </c>
       <c r="AC10" s="2">
         <f>Table1[[#This Row],[iDataC]]/$G$14*$G$15</f>
-        <v>163379.23750000002</v>
+        <v>163379.20000000001</v>
       </c>
       <c r="AD10" s="2">
         <v>262579</v>
@@ -8322,11 +10190,11 @@
       </c>
       <c r="AH10" s="2">
         <f>SUM(Table1[[#This Row],[iDataC]],Table1[[#This Row],[iStart]],Table1[[#This Row],[iResult]])</f>
-        <v>2823757.916666667</v>
+        <v>2823757.666666667</v>
       </c>
       <c r="AI10" s="2">
         <f>Table1[[#This Row],[iTotalC]]/$G$14*$G$15</f>
-        <v>423563.68750000006</v>
+        <v>423563.65000000008</v>
       </c>
       <c r="AJ10" s="1">
         <f>Table1[BRAM]/280</f>
@@ -8649,23 +10517,34 @@
         <v>1119954</v>
       </c>
       <c r="R14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="T14" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="U14" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="S14" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="T14" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="U14" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="V14" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA14" s="2">
-        <f>AVERAGE(AA3:AA10)</f>
-        <v>1126586.75</v>
+        <v>53</v>
+      </c>
+      <c r="Y14" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z14" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC14" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:51" x14ac:dyDescent="0.25">
@@ -8698,8 +10577,8 @@
         <v>0.6762387445000001</v>
       </c>
       <c r="V15" s="6">
-        <f>2000/T15/1000</f>
-        <v>2.957535361980431</v>
+        <f t="shared" ref="V15:V27" si="0">2000/T15</f>
+        <v>2957.5353619804309</v>
       </c>
       <c r="AA15" s="2">
         <f>AVERAGE(AA2,AA11,AA12)</f>
@@ -8729,15 +10608,15 @@
         <v>0.30107733000000003</v>
       </c>
       <c r="V16" s="6">
-        <f t="shared" ref="V16:V27" si="0">2000/T16/1000</f>
-        <v>6.6428116656939915</v>
+        <f t="shared" si="0"/>
+        <v>6642.8116656939919</v>
       </c>
       <c r="AA16" s="2">
         <f>AA14-AA15</f>
-        <v>36777.083333333256</v>
+        <v>36777.333333333256</v>
       </c>
     </row>
-    <row r="17" spans="12:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="12:29" x14ac:dyDescent="0.25">
       <c r="L17" s="7">
         <f>AVERAGE(L14:L16)</f>
         <v>450825829.66666669</v>
@@ -8756,10 +10635,10 @@
       </c>
       <c r="V17" s="6">
         <f t="shared" si="0"/>
-        <v>1.4679677601089127</v>
+        <v>1467.9677601089127</v>
       </c>
     </row>
-    <row r="18" spans="12:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="12:29" x14ac:dyDescent="0.25">
       <c r="L18" s="4">
         <f>L17/G14</f>
         <v>0.6762387445000001</v>
@@ -8773,153 +10652,354 @@
         <v>1</v>
       </c>
       <c r="T18" s="5">
-        <f>V3*(1/$G$15)</f>
-        <v>1.31428085E-2</v>
+        <f>V3*(1/$G$15)*1000</f>
+        <v>13.142808500000001</v>
       </c>
       <c r="V18" s="6">
         <f t="shared" si="0"/>
-        <v>152.17447625444746</v>
+        <v>152.17447625444743</v>
+      </c>
+      <c r="Y18" s="5">
+        <f>P3/$G$15*1000</f>
+        <v>1.6451210000000001</v>
+      </c>
+      <c r="Z18" s="5">
+        <f>R3/$G$15*1000</f>
+        <v>0.40040249999999999</v>
+      </c>
+      <c r="AA18" s="5">
+        <f t="shared" ref="Z18:AC18" si="1">R3/$G$15</f>
+        <v>4.0040250000000001E-4</v>
+      </c>
+      <c r="AB18" s="5">
+        <f t="shared" si="1"/>
+        <v>7.3981900000000003E-2</v>
+      </c>
+      <c r="AC18" s="5">
+        <f>T3/$G$15*1000</f>
+        <v>11.097284999999999</v>
       </c>
     </row>
-    <row r="19" spans="12:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="12:29" x14ac:dyDescent="0.25">
       <c r="L19" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M19" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="R19" s="2">
         <f>A4</f>
         <v>2</v>
       </c>
       <c r="T19" s="5">
-        <f t="shared" ref="T19:T27" si="1">V4*(1/$G$15)</f>
-        <v>7.8995390000000006E-3</v>
+        <f t="shared" ref="T19:T27" si="2">V4*(1/$G$15)*1000</f>
+        <v>7.8995390000000008</v>
       </c>
       <c r="V19" s="6">
         <f t="shared" si="0"/>
         <v>253.17933109767543</v>
       </c>
+      <c r="Y19" s="5">
+        <f t="shared" ref="Y19:Y27" si="3">P4/$G$15*1000</f>
+        <v>1.6441805000000003</v>
+      </c>
+      <c r="Z19" s="5">
+        <f t="shared" ref="Z19:Z27" si="4">R4/$G$15*1000</f>
+        <v>0.40118250000000011</v>
+      </c>
+      <c r="AA19" s="5">
+        <f t="shared" ref="AA19:AA27" si="5">R4/$G$15</f>
+        <v>4.011825000000001E-4</v>
+      </c>
+      <c r="AB19" s="5">
+        <f t="shared" ref="AB19:AB27" si="6">S4/$G$15</f>
+        <v>3.9027840000000001E-2</v>
+      </c>
+      <c r="AC19" s="5">
+        <f t="shared" ref="AC19:AC27" si="7">T4/$G$15*1000</f>
+        <v>5.8541759999999998</v>
+      </c>
     </row>
-    <row r="20" spans="12:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="12:29" x14ac:dyDescent="0.25">
       <c r="R20" s="2">
         <f>A5</f>
         <v>3</v>
       </c>
       <c r="T20" s="5">
-        <f t="shared" si="1"/>
-        <v>6.031718000000001E-3</v>
+        <f t="shared" si="2"/>
+        <v>6.0317180000000006</v>
       </c>
       <c r="V20" s="6">
         <f t="shared" si="0"/>
-        <v>331.58048834511152</v>
+        <v>331.58048834511158</v>
+      </c>
+      <c r="Y20" s="5">
+        <f t="shared" si="3"/>
+        <v>1.6447400000000001</v>
+      </c>
+      <c r="Z20" s="5">
+        <f t="shared" si="4"/>
+        <v>0.40066200000000002</v>
+      </c>
+      <c r="AA20" s="5">
+        <f t="shared" si="5"/>
+        <v>4.0066200000000003E-4</v>
+      </c>
+      <c r="AB20" s="5">
+        <f t="shared" si="6"/>
+        <v>2.6575439999999999E-2</v>
+      </c>
+      <c r="AC20" s="5">
+        <f t="shared" si="7"/>
+        <v>3.986316</v>
       </c>
     </row>
-    <row r="21" spans="12:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="12:29" x14ac:dyDescent="0.25">
       <c r="R21" s="2">
         <f>A6</f>
         <v>4</v>
       </c>
       <c r="T21" s="5">
-        <f t="shared" si="1"/>
-        <v>5.1845225000000002E-3</v>
+        <f t="shared" si="2"/>
+        <v>5.1845224999999999</v>
       </c>
       <c r="V21" s="6">
         <f t="shared" si="0"/>
-        <v>385.76358767851809</v>
+        <v>385.76358767851815</v>
+      </c>
+      <c r="Y21" s="5">
+        <f t="shared" si="3"/>
+        <v>1.6450835000000001</v>
+      </c>
+      <c r="Z21" s="5">
+        <f t="shared" si="4"/>
+        <v>0.40116000000000002</v>
+      </c>
+      <c r="AA21" s="5">
+        <f t="shared" si="5"/>
+        <v>4.0116000000000001E-4</v>
+      </c>
+      <c r="AB21" s="5">
+        <f t="shared" si="6"/>
+        <v>2.092186E-2</v>
+      </c>
+      <c r="AC21" s="5">
+        <f t="shared" si="7"/>
+        <v>3.1382790000000003</v>
       </c>
     </row>
-    <row r="22" spans="12:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="12:29" x14ac:dyDescent="0.25">
       <c r="R22" s="2">
         <f>A7</f>
         <v>5</v>
       </c>
       <c r="T22" s="5">
-        <f t="shared" si="1"/>
-        <v>4.6715554999999997E-3</v>
+        <f t="shared" si="2"/>
+        <v>4.6715554999999993</v>
       </c>
       <c r="V22" s="6">
         <f t="shared" si="0"/>
         <v>428.12292393829</v>
       </c>
+      <c r="Y22" s="5">
+        <f t="shared" si="3"/>
+        <v>1.6452665</v>
+      </c>
+      <c r="Z22" s="5">
+        <f t="shared" si="4"/>
+        <v>0.40041450000000006</v>
+      </c>
+      <c r="AA22" s="5">
+        <f t="shared" si="5"/>
+        <v>4.0041450000000004E-4</v>
+      </c>
+      <c r="AB22" s="5">
+        <f t="shared" si="6"/>
+        <v>1.750583E-2</v>
+      </c>
+      <c r="AC22" s="5">
+        <f t="shared" si="7"/>
+        <v>2.6258745000000001</v>
+      </c>
     </row>
-    <row r="23" spans="12:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="12:29" x14ac:dyDescent="0.25">
       <c r="R23" s="2">
         <f>A8</f>
         <v>6</v>
       </c>
       <c r="T23" s="5">
-        <f t="shared" si="1"/>
-        <v>4.3301284999999997E-3</v>
+        <f t="shared" si="2"/>
+        <v>4.3301284999999998</v>
       </c>
       <c r="V23" s="6">
         <f t="shared" si="0"/>
         <v>461.88005737012196</v>
       </c>
+      <c r="Y23" s="5">
+        <f t="shared" si="3"/>
+        <v>1.6442419999999998</v>
+      </c>
+      <c r="Z23" s="5">
+        <f t="shared" si="4"/>
+        <v>0.40090050000000005</v>
+      </c>
+      <c r="AA23" s="5">
+        <f t="shared" si="5"/>
+        <v>4.0090050000000005E-4</v>
+      </c>
+      <c r="AB23" s="5">
+        <f t="shared" si="6"/>
+        <v>1.523324E-2</v>
+      </c>
+      <c r="AC23" s="5">
+        <f t="shared" si="7"/>
+        <v>2.284986</v>
+      </c>
     </row>
-    <row r="24" spans="12:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="12:29" x14ac:dyDescent="0.25">
       <c r="R24" s="2">
         <f>A9</f>
         <v>7</v>
       </c>
       <c r="T24" s="5">
-        <f t="shared" si="1"/>
-        <v>4.1598469999999995E-3</v>
+        <f t="shared" si="2"/>
+        <v>4.1598469999999992</v>
       </c>
       <c r="V24" s="6">
         <f t="shared" si="0"/>
-        <v>480.78691355715733</v>
+        <v>480.78691355715739</v>
+      </c>
+      <c r="Y24" s="5">
+        <f t="shared" si="3"/>
+        <v>1.6441325</v>
+      </c>
+      <c r="Z24" s="5">
+        <f t="shared" si="4"/>
+        <v>0.40116450000000003</v>
+      </c>
+      <c r="AA24" s="5">
+        <f t="shared" si="5"/>
+        <v>4.0116450000000003E-4</v>
+      </c>
+      <c r="AB24" s="5">
+        <f t="shared" si="6"/>
+        <v>1.4097E-2</v>
+      </c>
+      <c r="AC24" s="5">
+        <f t="shared" si="7"/>
+        <v>2.1145500000000004</v>
       </c>
     </row>
-    <row r="25" spans="12:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="12:29" x14ac:dyDescent="0.25">
       <c r="R25" s="2">
         <f>A10</f>
         <v>8</v>
       </c>
       <c r="T25" s="5">
-        <f t="shared" si="1"/>
-        <v>3.9916774999999996E-3</v>
+        <f t="shared" si="2"/>
+        <v>3.9916774999999998</v>
       </c>
       <c r="V25" s="6">
         <f t="shared" si="0"/>
         <v>501.04248151309821</v>
       </c>
+      <c r="Y25" s="5">
+        <f t="shared" si="3"/>
+        <v>1.6453100000000001</v>
+      </c>
+      <c r="Z25" s="5">
+        <f t="shared" si="4"/>
+        <v>0.40083000000000002</v>
+      </c>
+      <c r="AA25" s="5">
+        <f t="shared" si="5"/>
+        <v>4.0083000000000002E-4</v>
+      </c>
+      <c r="AB25" s="5">
+        <f t="shared" si="6"/>
+        <v>1.2970249999999999E-2</v>
+      </c>
+      <c r="AC25" s="5">
+        <f t="shared" si="7"/>
+        <v>1.9455375000000004</v>
+      </c>
     </row>
-    <row r="26" spans="12:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="12:29" x14ac:dyDescent="0.25">
       <c r="R26" s="2">
         <f>A11</f>
         <v>9</v>
       </c>
       <c r="T26" s="5">
-        <f t="shared" si="1"/>
-        <v>3.7683300000000003E-3</v>
+        <f t="shared" si="2"/>
+        <v>3.7683300000000002</v>
       </c>
       <c r="V26" s="6">
         <f t="shared" si="0"/>
         <v>530.73908070683831</v>
       </c>
+      <c r="Y26" s="5">
+        <f t="shared" si="3"/>
+        <v>1.6442640000000004</v>
+      </c>
+      <c r="Z26" s="5">
+        <f t="shared" si="4"/>
+        <v>0.40022249999999998</v>
+      </c>
+      <c r="AA26" s="5">
+        <f t="shared" si="5"/>
+        <v>4.002225E-4</v>
+      </c>
+      <c r="AB26" s="5">
+        <f t="shared" si="6"/>
+        <v>1.149229E-2</v>
+      </c>
+      <c r="AC26" s="5">
+        <f t="shared" si="7"/>
+        <v>1.7238435000000001</v>
+      </c>
     </row>
-    <row r="27" spans="12:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="12:29" x14ac:dyDescent="0.25">
       <c r="R27" s="2">
         <f>A12</f>
         <v>10</v>
       </c>
       <c r="T27" s="5">
-        <f t="shared" si="1"/>
-        <v>3.6956040000000003E-3</v>
+        <f t="shared" si="2"/>
+        <v>3.6956040000000003</v>
       </c>
       <c r="V27" s="6">
         <f t="shared" si="0"/>
         <v>541.18352507465625</v>
+      </c>
+      <c r="Y27" s="5">
+        <f t="shared" si="3"/>
+        <v>1.6456589999999998</v>
+      </c>
+      <c r="Z27" s="5">
+        <f t="shared" si="4"/>
+        <v>0.39971550000000006</v>
+      </c>
+      <c r="AA27" s="5">
+        <f t="shared" si="5"/>
+        <v>3.9971550000000004E-4</v>
+      </c>
+      <c r="AB27" s="5">
+        <f t="shared" si="6"/>
+        <v>1.1001530000000001E-2</v>
+      </c>
+      <c r="AC27" s="5">
+        <f t="shared" si="7"/>
+        <v>1.6502295000000002</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="95" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>